<commit_message>
add slaughter animals to calculation
</commit_message>
<xml_diff>
--- a/data/input-table.xlsx
+++ b/data/input-table.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\larsc\Desktop\DA-job\DA-nutrient-flow-Kleve\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BDA83A-C84F-4344-B5E5-F1D61A44EA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF4E83C-0629-456E-9068-EE27B417F548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1E434030-2D60-46AB-AE5D-61B754A2590A}"/>
+    <workbookView xWindow="3624" yWindow="2316" windowWidth="13536" windowHeight="10044" activeTab="2" xr2:uid="{1E434030-2D60-46AB-AE5D-61B754A2590A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Input_Animal" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="200">
   <si>
     <t>description</t>
   </si>
@@ -310,13 +312,424 @@
   </si>
   <si>
     <t>local_vegetal_products</t>
+  </si>
+  <si>
+    <t>population</t>
+  </si>
+  <si>
+    <t>consume_wheat</t>
+  </si>
+  <si>
+    <t>consume_rye</t>
+  </si>
+  <si>
+    <t>consume_rice</t>
+  </si>
+  <si>
+    <t>consume_legumes</t>
+  </si>
+  <si>
+    <t>consume_potato</t>
+  </si>
+  <si>
+    <t>consume_potato_starch</t>
+  </si>
+  <si>
+    <t>consume_sugar</t>
+  </si>
+  <si>
+    <t>consume_honey</t>
+  </si>
+  <si>
+    <t>consume_cocoa</t>
+  </si>
+  <si>
+    <t>consume_tree_fruits</t>
+  </si>
+  <si>
+    <t>consume_citrus_fruits</t>
+  </si>
+  <si>
+    <t>consume_nuts</t>
+  </si>
+  <si>
+    <t>consume_dried_fruit</t>
+  </si>
+  <si>
+    <t>consume_vegetables</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>kg / person / year</t>
+  </si>
+  <si>
+    <t>persons</t>
+  </si>
+  <si>
+    <t>consume_beef</t>
+  </si>
+  <si>
+    <t>consume_pork</t>
+  </si>
+  <si>
+    <t>consume_sheep</t>
+  </si>
+  <si>
+    <t>consume_offal</t>
+  </si>
+  <si>
+    <t>consume_poultry</t>
+  </si>
+  <si>
+    <t>consume_other_meat</t>
+  </si>
+  <si>
+    <t>beef and veal</t>
+  </si>
+  <si>
+    <t>pork meat</t>
+  </si>
+  <si>
+    <t>sheep and goat meat</t>
+  </si>
+  <si>
+    <t>offal</t>
+  </si>
+  <si>
+    <t>poultry</t>
+  </si>
+  <si>
+    <t>other meat (game, rabbit)</t>
+  </si>
+  <si>
+    <t>fish and fish products (catch weight)</t>
+  </si>
+  <si>
+    <t>fresh milk products</t>
+  </si>
+  <si>
+    <t>cream</t>
+  </si>
+  <si>
+    <t>condensed milk (product weight)</t>
+  </si>
+  <si>
+    <t>cheese incl. Cheese spread (product weight)</t>
+  </si>
+  <si>
+    <t>butter (product weight)</t>
+  </si>
+  <si>
+    <t>vegetable fats (clarified)</t>
+  </si>
+  <si>
+    <t>consume_fish</t>
+  </si>
+  <si>
+    <t>consume_milk</t>
+  </si>
+  <si>
+    <t>consume_cream</t>
+  </si>
+  <si>
+    <t>consume_condensed_milk</t>
+  </si>
+  <si>
+    <t>consume_cheese</t>
+  </si>
+  <si>
+    <t>consume_butter</t>
+  </si>
+  <si>
+    <t>consume_vegetable_fat</t>
+  </si>
+  <si>
+    <t>margarine</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">food oil </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>49</t>
+    </r>
+  </si>
+  <si>
+    <t>egg</t>
+  </si>
+  <si>
+    <t>consume_margarine</t>
+  </si>
+  <si>
+    <t>cosume_food_oil</t>
+  </si>
+  <si>
+    <t>consume_egg</t>
+  </si>
+  <si>
+    <t>g N / 100 gram product</t>
+  </si>
+  <si>
+    <t>N_content_wheat</t>
+  </si>
+  <si>
+    <t>N_content_rye</t>
+  </si>
+  <si>
+    <t>N_content_rice</t>
+  </si>
+  <si>
+    <t>N_content_legumes</t>
+  </si>
+  <si>
+    <t>N_content_potato</t>
+  </si>
+  <si>
+    <t>N_content_potato_starch</t>
+  </si>
+  <si>
+    <t>N_content_sugar</t>
+  </si>
+  <si>
+    <t>N_content_honey</t>
+  </si>
+  <si>
+    <t>N_content_cocoa</t>
+  </si>
+  <si>
+    <t>N_content_tree_fruits</t>
+  </si>
+  <si>
+    <t>N_content_citrus_fruits</t>
+  </si>
+  <si>
+    <t>N_content_nuts</t>
+  </si>
+  <si>
+    <t>N_content_dried_fruit</t>
+  </si>
+  <si>
+    <t>N_content_vegetables</t>
+  </si>
+  <si>
+    <t>N_content_beef</t>
+  </si>
+  <si>
+    <t>N_content_pork</t>
+  </si>
+  <si>
+    <t>N_content_sheep</t>
+  </si>
+  <si>
+    <t>N_contente_offal</t>
+  </si>
+  <si>
+    <t>N_content_poultry</t>
+  </si>
+  <si>
+    <t>N_content_other_meat</t>
+  </si>
+  <si>
+    <t>N_content_fish</t>
+  </si>
+  <si>
+    <t>N_content_milk</t>
+  </si>
+  <si>
+    <t>N_content_cream</t>
+  </si>
+  <si>
+    <t>N_content_condensed_milk</t>
+  </si>
+  <si>
+    <t>N_content_cheese</t>
+  </si>
+  <si>
+    <t>N_content_butter</t>
+  </si>
+  <si>
+    <t>N_content_margarine</t>
+  </si>
+  <si>
+    <t>N_content_egg</t>
+  </si>
+  <si>
+    <r>
+      <t>Dairy cattle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 4</t>
+    </r>
+  </si>
+  <si>
+    <t>Oxes</t>
+  </si>
+  <si>
+    <t>Bulls</t>
+  </si>
+  <si>
+    <t>Female cattle (before calving)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Younstock </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>≤ 8 months</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Younstock </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>≥ 8 and ≤</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 12 months 15</t>
+    </r>
+  </si>
+  <si>
+    <t>slaughter_weight_oxes</t>
+  </si>
+  <si>
+    <t>slaughter_weight_bulls</t>
+  </si>
+  <si>
+    <t>slaughter_weight_female_cattle</t>
+  </si>
+  <si>
+    <t>slaughter_weight_younstock_midage</t>
+  </si>
+  <si>
+    <t>slaughter_weight_younstock_youngage</t>
+  </si>
+  <si>
+    <t>slaughter_weight_dairy_cattle</t>
+  </si>
+  <si>
+    <t>number_slaughter_dairy_cattle</t>
+  </si>
+  <si>
+    <t>number_slaughter_oxes</t>
+  </si>
+  <si>
+    <t>number_slaughter_bulls</t>
+  </si>
+  <si>
+    <t>number_slaughter_female_cattle</t>
+  </si>
+  <si>
+    <t>number_slaughter_younstock_youngage</t>
+  </si>
+  <si>
+    <t>number_slaughter_younstock_midage</t>
+  </si>
+  <si>
+    <t>number_slaughter_pig</t>
+  </si>
+  <si>
+    <t>number_slaughter_poultry</t>
+  </si>
+  <si>
+    <t>number_slaughter_sheep</t>
+  </si>
+  <si>
+    <t>number_slaughter_lamb</t>
+  </si>
+  <si>
+    <t>number_slaughter_goat</t>
+  </si>
+  <si>
+    <t>number_slaughter_horse</t>
+  </si>
+  <si>
+    <t>slaughter_weight_pig</t>
+  </si>
+  <si>
+    <t>slaughter_weight_poultry</t>
+  </si>
+  <si>
+    <t>slaughter_weight_lamb</t>
+  </si>
+  <si>
+    <t>slaughter_weight_sheep</t>
+  </si>
+  <si>
+    <t>slaughter_weight_goat</t>
+  </si>
+  <si>
+    <t>slaughter_weight_horse</t>
+  </si>
+  <si>
+    <t>edible_fraction_cattle</t>
+  </si>
+  <si>
+    <t>edible_fraction_pig</t>
+  </si>
+  <si>
+    <t>edible_fraction_poultry</t>
+  </si>
+  <si>
+    <t>edible_fraction_other</t>
+  </si>
+  <si>
+    <t>N_content_female_cattle</t>
+  </si>
+  <si>
+    <t>N_content_male_cattle</t>
+  </si>
+  <si>
+    <t>N_content_pig</t>
+  </si>
+  <si>
+    <t>N_content_horse</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,10 +745,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -365,10 +785,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -703,8 +1165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05448A46-9CD3-4A05-BF5C-7BD7F4966E0F}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1741,4 +2203,1096 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72EBF83B-C21A-4566-828D-A96EF21607E8}">
+  <dimension ref="A1:G60"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="A1:G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="33" style="8" customWidth="1"/>
+    <col min="3" max="3" width="21.21875" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" style="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="10">
+        <v>310329</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" s="7">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" s="7">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E6" s="7">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E7" s="11">
+        <v>57.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="7">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" s="7">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" s="7">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" t="s">
+        <v>99</v>
+      </c>
+      <c r="E11" s="7">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" s="7">
+        <v>65.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E13" s="7">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" t="s">
+        <v>99</v>
+      </c>
+      <c r="E14" s="7">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" t="s">
+        <v>99</v>
+      </c>
+      <c r="E15" s="7">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" s="7">
+        <v>98.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" s="12">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" s="12">
+        <v>50.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19" s="12">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" s="12">
+        <v>20.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C22" t="s">
+        <v>99</v>
+      </c>
+      <c r="E22" s="12">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C23" t="s">
+        <v>99</v>
+      </c>
+      <c r="E23" s="12">
+        <v>14.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C24" t="s">
+        <v>99</v>
+      </c>
+      <c r="E24" s="12">
+        <v>83.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C25" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C26" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" s="12">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C27" t="s">
+        <v>99</v>
+      </c>
+      <c r="E27" s="12">
+        <v>24.7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28" t="s">
+        <v>99</v>
+      </c>
+      <c r="E28" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C29" t="s">
+        <v>99</v>
+      </c>
+      <c r="E29" s="12">
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C30" t="s">
+        <v>99</v>
+      </c>
+      <c r="E30" s="12">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E31" s="12">
+        <v>11.7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="C32" t="s">
+        <v>99</v>
+      </c>
+      <c r="E32" s="13">
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E33">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E34">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E35">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E36">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E37" s="14">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E38" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E40">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E41">
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E42" s="15">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E43">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E44">
+        <v>4.76</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C45" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E45">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E46">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E47">
+        <v>3.39</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E48">
+        <v>3.52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E49">
+        <v>3.26</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E50" s="15">
+        <v>2.38</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E51">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C52" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E52">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E53">
+        <v>2.67</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C54" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E54">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C55" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E55">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C56" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E56">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E57" s="3">
+        <v>4.1399999999999997</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E58">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E59">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E60" s="3">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76B6A283-D1DF-47BA-930D-AF74861CE3AB}">
+  <dimension ref="A1:G35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E2" s="3">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="E3" s="3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="E4" s="3">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>178</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="E6" s="3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>179</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E7" s="3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>180</v>
+      </c>
+      <c r="E8">
+        <v>723164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>181</v>
+      </c>
+      <c r="E9">
+        <v>2101.4858623891359</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>183</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>182</v>
+      </c>
+      <c r="E11" s="3">
+        <v>2242</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>184</v>
+      </c>
+      <c r="E12" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>185</v>
+      </c>
+      <c r="E13" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>173</v>
+      </c>
+      <c r="B14" t="s">
+        <v>162</v>
+      </c>
+      <c r="E14" s="3">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>168</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="E15" s="3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>169</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="E16" s="3">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>170</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>172</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="E18" s="3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>171</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E19" s="3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>186</v>
+      </c>
+      <c r="E20">
+        <v>96.303174200810403</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>187</v>
+      </c>
+      <c r="E21">
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>188</v>
+      </c>
+      <c r="E22">
+        <v>18.002070393374741</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>189</v>
+      </c>
+      <c r="E23">
+        <v>29.992229992229991</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>190</v>
+      </c>
+      <c r="E24">
+        <v>17.761989342806395</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>191</v>
+      </c>
+      <c r="E25">
+        <v>264.04800872885977</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>192</v>
+      </c>
+      <c r="E26" s="15">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>193</v>
+      </c>
+      <c r="E27" s="9">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>194</v>
+      </c>
+      <c r="E28" s="9">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>195</v>
+      </c>
+      <c r="E29">
+        <v>0.55500000000000005</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>196</v>
+      </c>
+      <c r="E30" s="20">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>197</v>
+      </c>
+      <c r="E31" s="18">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>198</v>
+      </c>
+      <c r="E32">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>152</v>
+      </c>
+      <c r="E33" s="15">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>150</v>
+      </c>
+      <c r="E34" s="15">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>199</v>
+      </c>
+      <c r="E35" s="15">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added modelling of crop N yields
</commit_message>
<xml_diff>
--- a/data/input-table.xlsx
+++ b/data/input-table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\larsc\Desktop\DA-job\DA-nutrient-flow-Kleve\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF4E83C-0629-456E-9068-EE27B417F548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79803703-CB66-4D10-ACDF-3D65734F2937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3624" yWindow="2316" windowWidth="13536" windowHeight="10044" activeTab="2" xr2:uid="{1E434030-2D60-46AB-AE5D-61B754A2590A}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="13536" windowHeight="10044" activeTab="2" xr2:uid="{1E434030-2D60-46AB-AE5D-61B754A2590A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="268">
   <si>
     <t>description</t>
   </si>
@@ -563,21 +563,6 @@
     <t>N_content_egg</t>
   </si>
   <si>
-    <r>
-      <t>Dairy cattle</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 4</t>
-    </r>
-  </si>
-  <si>
     <t>Oxes</t>
   </si>
   <si>
@@ -587,44 +572,6 @@
     <t>Female cattle (before calving)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Younstock </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>≤ 8 months</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Younstock </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>≥ 8 and ≤</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 12 months 15</t>
-    </r>
-  </si>
-  <si>
     <t>slaughter_weight_oxes</t>
   </si>
   <si>
@@ -643,42 +590,6 @@
     <t>slaughter_weight_dairy_cattle</t>
   </si>
   <si>
-    <t>number_slaughter_dairy_cattle</t>
-  </si>
-  <si>
-    <t>number_slaughter_oxes</t>
-  </si>
-  <si>
-    <t>number_slaughter_bulls</t>
-  </si>
-  <si>
-    <t>number_slaughter_female_cattle</t>
-  </si>
-  <si>
-    <t>number_slaughter_younstock_youngage</t>
-  </si>
-  <si>
-    <t>number_slaughter_younstock_midage</t>
-  </si>
-  <si>
-    <t>number_slaughter_pig</t>
-  </si>
-  <si>
-    <t>number_slaughter_poultry</t>
-  </si>
-  <si>
-    <t>number_slaughter_sheep</t>
-  </si>
-  <si>
-    <t>number_slaughter_lamb</t>
-  </si>
-  <si>
-    <t>number_slaughter_goat</t>
-  </si>
-  <si>
-    <t>number_slaughter_horse</t>
-  </si>
-  <si>
     <t>slaughter_weight_pig</t>
   </si>
   <si>
@@ -719,17 +630,265 @@
   </si>
   <si>
     <t>N_content_horse</t>
+  </si>
+  <si>
+    <t>Dairy cattle 4</t>
+  </si>
+  <si>
+    <t>n_slaughter_dairy_cattle</t>
+  </si>
+  <si>
+    <t>individuals</t>
+  </si>
+  <si>
+    <t>n_slaughter_oxes</t>
+  </si>
+  <si>
+    <t>n_slaughter_bulls</t>
+  </si>
+  <si>
+    <t>n_slaughter_female_cattle</t>
+  </si>
+  <si>
+    <t>Younstock ≤ 8 months</t>
+  </si>
+  <si>
+    <t>n_slaughter_younstock_youngage</t>
+  </si>
+  <si>
+    <t>Younstock ≥ 8 and ≤ 12 months 15</t>
+  </si>
+  <si>
+    <t>n_slaughter_younstock_midage</t>
+  </si>
+  <si>
+    <t>n_slaughter_pig</t>
+  </si>
+  <si>
+    <t>n_slaughter_poultry</t>
+  </si>
+  <si>
+    <t>n_slaughter_lamb</t>
+  </si>
+  <si>
+    <t>n_slaughter_sheep</t>
+  </si>
+  <si>
+    <t>n_slaughter_goat</t>
+  </si>
+  <si>
+    <t>n_slaughter_horse</t>
+  </si>
+  <si>
+    <t>n_slaughter_import_dairy_cattle</t>
+  </si>
+  <si>
+    <t>n_slaughter_import_oxes</t>
+  </si>
+  <si>
+    <t>n_slaughter_import_bulls</t>
+  </si>
+  <si>
+    <t>n_slaughter_import_female_cattle</t>
+  </si>
+  <si>
+    <t>n_slaughter_import_younstock_youngage</t>
+  </si>
+  <si>
+    <t>n_slaughter_import_younstock_midage</t>
+  </si>
+  <si>
+    <t>n_slaughter_import_pig</t>
+  </si>
+  <si>
+    <t>n_slaughter_import_poultry</t>
+  </si>
+  <si>
+    <t>n_slaughter_import_lamb</t>
+  </si>
+  <si>
+    <t>n_slaughter_import_sheep</t>
+  </si>
+  <si>
+    <t>n_slaughter_import_goat</t>
+  </si>
+  <si>
+    <t>n_slaughter_import_horse</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>slaughter_weight_fraction_cattle</t>
+  </si>
+  <si>
+    <t>slaughter_weight_fraction_pig</t>
+  </si>
+  <si>
+    <t>slaughter_weight_fraction_poultry</t>
+  </si>
+  <si>
+    <t>slaughter_weight_fraction_others</t>
+  </si>
+  <si>
+    <t>gr N / 100 gram product</t>
+  </si>
+  <si>
+    <t>egg laying rate (consumable eggs)</t>
+  </si>
+  <si>
+    <t>egg_per_chicken</t>
+  </si>
+  <si>
+    <t>egg per chicken</t>
+  </si>
+  <si>
+    <t>weight of average egg</t>
+  </si>
+  <si>
+    <t>egg-weight</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>calculated based on total milk</t>
+  </si>
+  <si>
+    <t>share_milk_to_factory</t>
+  </si>
+  <si>
+    <t>share_milk_fed_farm</t>
+  </si>
+  <si>
+    <t>share_milk_direct_sale</t>
+  </si>
+  <si>
+    <t>share_milk_other_use</t>
+  </si>
+  <si>
+    <t>taken IT.NRW for 2016</t>
+  </si>
+  <si>
+    <t>n_dairy_cow</t>
+  </si>
+  <si>
+    <t>calculated based on cow number and milk output</t>
+  </si>
+  <si>
+    <t>milk_per_cow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kg per cow </t>
+  </si>
+  <si>
+    <t>calculated on LLU units in Nährstoffreport</t>
+  </si>
+  <si>
+    <t>n_other_poultry</t>
+  </si>
+  <si>
+    <t>weeks until turkey is slaughtered</t>
+  </si>
+  <si>
+    <t>weeks_to_grow</t>
+  </si>
+  <si>
+    <t>weeks</t>
+  </si>
+  <si>
+    <t>n_hens</t>
+  </si>
+  <si>
+    <t>number of egg-laying hens in Kleve (assuming that the number of eggs in correct)</t>
+  </si>
+  <si>
+    <t>n_bull</t>
+  </si>
+  <si>
+    <t>n_heifer</t>
+  </si>
+  <si>
+    <t>n_calf</t>
+  </si>
+  <si>
+    <t>n_pig</t>
+  </si>
+  <si>
+    <t>all_non-egg-laying poultry</t>
+  </si>
+  <si>
+    <t>n_rooster</t>
+  </si>
+  <si>
+    <t>n_sheep</t>
+  </si>
+  <si>
+    <t>N_excrement_rate_dairy</t>
+  </si>
+  <si>
+    <t>N_excrement_rate_bull</t>
+  </si>
+  <si>
+    <t>N_excrement_rate_heifer</t>
+  </si>
+  <si>
+    <t>N_excrement_rate_calf</t>
+  </si>
+  <si>
+    <t>N_excrement_rate_pig</t>
+  </si>
+  <si>
+    <t>N_excrement_rate_hen</t>
+  </si>
+  <si>
+    <t>N_excrement_rate_rooster</t>
+  </si>
+  <si>
+    <t>N_excrement_rate_sheep</t>
+  </si>
+  <si>
+    <t>kg N per animal per year</t>
+  </si>
+  <si>
+    <t>N_housingloss_rate_cattle_liquid</t>
+  </si>
+  <si>
+    <t>N_housingloss_rate_pig_liquid</t>
+  </si>
+  <si>
+    <t>N_housingloss_rate_cattle_solid</t>
+  </si>
+  <si>
+    <t>share</t>
+  </si>
+  <si>
+    <t>share_liquid_excrement_cattle</t>
+  </si>
+  <si>
+    <t>share_liquid_excrement_pig</t>
+  </si>
+  <si>
+    <t>loss rate of N from total manure</t>
+  </si>
+  <si>
+    <t>rate of cattles kept on liquid manure catchment systems</t>
+  </si>
+  <si>
+    <t>manure_to_biogas</t>
+  </si>
+  <si>
+    <t>kg N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -750,12 +909,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -785,7 +938,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -824,13 +977,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2949,24 +3095,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76B6A283-D1DF-47BA-930D-AF74861CE3AB}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="B61" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>98</v>
@@ -2974,7 +3121,7 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
       <c r="F1" t="s">
@@ -2986,310 +3133,989 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="B2" t="s">
-        <v>162</v>
-      </c>
-      <c r="E2" s="3">
+        <v>186</v>
+      </c>
+      <c r="C2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E2">
         <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="E3" s="3">
+        <v>162</v>
+      </c>
+      <c r="B3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E3">
         <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>176</v>
-      </c>
-      <c r="B4" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="B4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E4">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>164</v>
       </c>
-      <c r="E4" s="3">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>177</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>165</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="B5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E5">
         <v>1404</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>178</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="E6" s="3">
+        <v>191</v>
+      </c>
+      <c r="B6" t="s">
+        <v>192</v>
+      </c>
+      <c r="C6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E6">
         <v>177</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>179</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="E7" s="3">
+        <v>193</v>
+      </c>
+      <c r="B7" t="s">
+        <v>194</v>
+      </c>
+      <c r="C7" t="s">
+        <v>187</v>
+      </c>
+      <c r="E7">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>180</v>
+      <c r="B8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C8" t="s">
+        <v>187</v>
       </c>
       <c r="E8">
         <v>723164</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>181</v>
+      <c r="B9" t="s">
+        <v>196</v>
+      </c>
+      <c r="C9" t="s">
+        <v>187</v>
       </c>
       <c r="E9">
-        <v>2101.4858623891359</v>
+        <v>2101</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>183</v>
-      </c>
-      <c r="E10" s="3">
+      <c r="B10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C10" t="s">
+        <v>187</v>
+      </c>
+      <c r="E10">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>182</v>
-      </c>
-      <c r="E11" s="3">
+      <c r="B11" t="s">
+        <v>198</v>
+      </c>
+      <c r="C11" t="s">
+        <v>187</v>
+      </c>
+      <c r="E11">
         <v>2242</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>184</v>
-      </c>
-      <c r="E12" s="3">
+      <c r="B12" t="s">
+        <v>199</v>
+      </c>
+      <c r="C12" t="s">
+        <v>187</v>
+      </c>
+      <c r="E12">
         <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>185</v>
-      </c>
-      <c r="E13" s="3">
+      <c r="B13" t="s">
+        <v>200</v>
+      </c>
+      <c r="C13" t="s">
+        <v>187</v>
+      </c>
+      <c r="E13">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>173</v>
-      </c>
       <c r="B14" t="s">
-        <v>162</v>
-      </c>
-      <c r="E14" s="3">
-        <v>254</v>
+        <v>201</v>
+      </c>
+      <c r="C14" t="s">
+        <v>187</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>168</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="E15" s="3">
-        <v>94</v>
+      <c r="B15" t="s">
+        <v>202</v>
+      </c>
+      <c r="C15" t="s">
+        <v>187</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>169</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="E16" s="3">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>170</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>165</v>
-      </c>
-      <c r="E17" s="3">
-        <v>1404</v>
+      <c r="B16" t="s">
+        <v>203</v>
+      </c>
+      <c r="C16" t="s">
+        <v>187</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>204</v>
+      </c>
+      <c r="C17" t="s">
+        <v>187</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>172</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="E18" s="3">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>171</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="E19" s="3">
-        <v>28</v>
+      <c r="B18" t="s">
+        <v>205</v>
+      </c>
+      <c r="C18" t="s">
+        <v>187</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>206</v>
+      </c>
+      <c r="C19" t="s">
+        <v>187</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>186</v>
+      <c r="B20" t="s">
+        <v>207</v>
+      </c>
+      <c r="C20" t="s">
+        <v>187</v>
       </c>
       <c r="E20">
-        <v>96.303174200810403</v>
+        <v>142865</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
+        <v>208</v>
+      </c>
+      <c r="C21" t="s">
         <v>187</v>
       </c>
       <c r="E21">
-        <v>2.13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>188</v>
+      <c r="B22" t="s">
+        <v>209</v>
+      </c>
+      <c r="C22" t="s">
+        <v>187</v>
       </c>
       <c r="E22">
-        <v>18.002070393374741</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>189</v>
+      <c r="B23" t="s">
+        <v>210</v>
+      </c>
+      <c r="C23" t="s">
+        <v>187</v>
       </c>
       <c r="E23">
-        <v>29.992229992229991</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>190</v>
+      <c r="B24" t="s">
+        <v>211</v>
+      </c>
+      <c r="C24" t="s">
+        <v>187</v>
       </c>
       <c r="E24">
-        <v>17.761989342806395</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>191</v>
+      <c r="B25" t="s">
+        <v>212</v>
+      </c>
+      <c r="C25" t="s">
+        <v>187</v>
       </c>
       <c r="E25">
-        <v>264.04800872885977</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>192</v>
-      </c>
-      <c r="E26" s="15">
-        <v>0.52</v>
+        <v>185</v>
+      </c>
+      <c r="B26" t="s">
+        <v>170</v>
+      </c>
+      <c r="C26" t="s">
+        <v>213</v>
+      </c>
+      <c r="E26">
+        <v>290.8940106</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>193</v>
-      </c>
-      <c r="E27" s="9">
-        <v>0.68</v>
+        <v>162</v>
+      </c>
+      <c r="B27" t="s">
+        <v>165</v>
+      </c>
+      <c r="C27" t="s">
+        <v>213</v>
+      </c>
+      <c r="E27">
+        <v>340.16093640000003</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>194</v>
-      </c>
-      <c r="E28" s="9">
-        <v>0.64</v>
+        <v>163</v>
+      </c>
+      <c r="B28" t="s">
+        <v>166</v>
+      </c>
+      <c r="C28" t="s">
+        <v>213</v>
+      </c>
+      <c r="E28">
+        <v>401.14754360000001</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>195</v>
+        <v>164</v>
+      </c>
+      <c r="B29" t="s">
+        <v>167</v>
+      </c>
+      <c r="C29" t="s">
+        <v>213</v>
       </c>
       <c r="E29">
-        <v>0.55500000000000005</v>
+        <v>271.15635359999999</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>196</v>
-      </c>
-      <c r="E30" s="20">
-        <v>2.5</v>
+        <v>191</v>
+      </c>
+      <c r="B30" t="s">
+        <v>169</v>
+      </c>
+      <c r="C30" t="s">
+        <v>213</v>
+      </c>
+      <c r="E30">
+        <v>151.07069730000001</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>197</v>
-      </c>
-      <c r="E31" s="18">
+        <v>193</v>
+      </c>
+      <c r="B31" t="s">
+        <v>168</v>
+      </c>
+      <c r="C31" t="s">
+        <v>213</v>
+      </c>
+      <c r="E31">
+        <v>176.4484928</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>171</v>
+      </c>
+      <c r="C32" t="s">
+        <v>213</v>
+      </c>
+      <c r="E32">
+        <v>96.303174200000001</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>172</v>
+      </c>
+      <c r="C33" t="s">
+        <v>213</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>173</v>
+      </c>
+      <c r="C34" t="s">
+        <v>213</v>
+      </c>
+      <c r="E34">
+        <v>18.00207039</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>174</v>
+      </c>
+      <c r="C35" t="s">
+        <v>213</v>
+      </c>
+      <c r="E35">
+        <v>29.992229989999998</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>175</v>
+      </c>
+      <c r="C36" t="s">
+        <v>213</v>
+      </c>
+      <c r="E36">
+        <v>17.76198934</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>176</v>
+      </c>
+      <c r="C37" t="s">
+        <v>213</v>
+      </c>
+      <c r="E37">
+        <v>264.04800870000003</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>214</v>
+      </c>
+      <c r="E38">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>215</v>
+      </c>
+      <c r="E39">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>216</v>
+      </c>
+      <c r="E40">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>217</v>
+      </c>
+      <c r="E41">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>177</v>
+      </c>
+      <c r="E42">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>178</v>
+      </c>
+      <c r="E43">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>179</v>
+      </c>
+      <c r="E44">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>180</v>
+      </c>
+      <c r="E45">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>181</v>
+      </c>
+      <c r="C46" t="s">
+        <v>218</v>
+      </c>
+      <c r="E46">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>182</v>
+      </c>
+      <c r="C47" t="s">
+        <v>218</v>
+      </c>
+      <c r="E47">
         <v>2.7</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>198</v>
-      </c>
-      <c r="E32">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>183</v>
+      </c>
+      <c r="C48" t="s">
+        <v>218</v>
+      </c>
+      <c r="E48">
         <v>2.56</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
         <v>152</v>
       </c>
-      <c r="E33" s="15">
+      <c r="C49" t="s">
+        <v>218</v>
+      </c>
+      <c r="E49">
         <v>3.25</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
         <v>150</v>
       </c>
-      <c r="E34" s="15">
+      <c r="C50" t="s">
+        <v>218</v>
+      </c>
+      <c r="E50">
         <v>2.6</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>199</v>
-      </c>
-      <c r="E35" s="15">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>184</v>
+      </c>
+      <c r="C51" t="s">
+        <v>218</v>
+      </c>
+      <c r="E51">
         <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>219</v>
+      </c>
+      <c r="B52" t="s">
+        <v>220</v>
+      </c>
+      <c r="C52" t="s">
+        <v>221</v>
+      </c>
+      <c r="E52">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>222</v>
+      </c>
+      <c r="B53" t="s">
+        <v>223</v>
+      </c>
+      <c r="C53" t="s">
+        <v>224</v>
+      </c>
+      <c r="E53">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>218</v>
+      </c>
+      <c r="B54" t="s">
+        <v>161</v>
+      </c>
+      <c r="C54" t="s">
+        <v>218</v>
+      </c>
+      <c r="E54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>225</v>
+      </c>
+      <c r="B55" t="s">
+        <v>155</v>
+      </c>
+      <c r="C55" t="s">
+        <v>218</v>
+      </c>
+      <c r="E55">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>225</v>
+      </c>
+      <c r="B56" t="s">
+        <v>226</v>
+      </c>
+      <c r="E56">
+        <v>0.76900000000000002</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>225</v>
+      </c>
+      <c r="B57" t="s">
+        <v>227</v>
+      </c>
+      <c r="E57">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>225</v>
+      </c>
+      <c r="B58" t="s">
+        <v>228</v>
+      </c>
+      <c r="E58">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>225</v>
+      </c>
+      <c r="B59" t="s">
+        <v>229</v>
+      </c>
+      <c r="E59">
+        <v>0.215</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>232</v>
+      </c>
+      <c r="B60" t="s">
+        <v>233</v>
+      </c>
+      <c r="C60" t="s">
+        <v>234</v>
+      </c>
+      <c r="E60">
+        <v>7671.4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>235</v>
+      </c>
+      <c r="B61" t="s">
+        <v>236</v>
+      </c>
+      <c r="C61" t="s">
+        <v>187</v>
+      </c>
+      <c r="E61">
+        <v>435440</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>237</v>
+      </c>
+      <c r="B62" t="s">
+        <v>238</v>
+      </c>
+      <c r="C62" t="s">
+        <v>239</v>
+      </c>
+      <c r="D62">
+        <v>19</v>
+      </c>
+      <c r="E62">
+        <v>20</v>
+      </c>
+      <c r="F62">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>230</v>
+      </c>
+      <c r="B63" t="s">
+        <v>231</v>
+      </c>
+      <c r="C63" t="s">
+        <v>187</v>
+      </c>
+      <c r="E63" s="3">
+        <v>56794</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
+        <v>242</v>
+      </c>
+      <c r="C64" t="s">
+        <v>187</v>
+      </c>
+      <c r="E64">
+        <v>7391</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>243</v>
+      </c>
+      <c r="C65" t="s">
+        <v>187</v>
+      </c>
+      <c r="E65">
+        <v>40838</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>244</v>
+      </c>
+      <c r="C66" t="s">
+        <v>187</v>
+      </c>
+      <c r="E66">
+        <v>24403</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
+        <v>245</v>
+      </c>
+      <c r="C67" t="s">
+        <v>187</v>
+      </c>
+      <c r="E67" s="3">
+        <v>365448</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>241</v>
+      </c>
+      <c r="B68" t="s">
+        <v>240</v>
+      </c>
+      <c r="C68" t="s">
+        <v>187</v>
+      </c>
+      <c r="E68">
+        <v>194946.33155188253</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>246</v>
+      </c>
+      <c r="B69" t="s">
+        <v>247</v>
+      </c>
+      <c r="C69" t="s">
+        <v>187</v>
+      </c>
+      <c r="E69">
+        <v>564535.90832480637</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>248</v>
+      </c>
+      <c r="C70" t="s">
+        <v>187</v>
+      </c>
+      <c r="E70">
+        <v>6121</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
+        <v>249</v>
+      </c>
+      <c r="D71">
+        <v>99.8</v>
+      </c>
+      <c r="F71">
+        <v>128.80000000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
+        <v>250</v>
+      </c>
+      <c r="C72" t="s">
+        <v>257</v>
+      </c>
+      <c r="E72">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B73" t="s">
+        <v>251</v>
+      </c>
+      <c r="C73" t="s">
+        <v>257</v>
+      </c>
+      <c r="E73">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
+        <v>252</v>
+      </c>
+      <c r="C74" t="s">
+        <v>257</v>
+      </c>
+      <c r="E74">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B75" t="s">
+        <v>253</v>
+      </c>
+      <c r="C75" t="s">
+        <v>257</v>
+      </c>
+      <c r="E75">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B76" t="s">
+        <v>254</v>
+      </c>
+      <c r="C76" t="s">
+        <v>257</v>
+      </c>
+      <c r="E76">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B77" t="s">
+        <v>255</v>
+      </c>
+      <c r="C77" t="s">
+        <v>257</v>
+      </c>
+      <c r="E77">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B78" t="s">
+        <v>256</v>
+      </c>
+      <c r="C78" t="s">
+        <v>257</v>
+      </c>
+      <c r="E78">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>264</v>
+      </c>
+      <c r="B79" t="s">
+        <v>258</v>
+      </c>
+      <c r="C79" t="s">
+        <v>261</v>
+      </c>
+      <c r="E79">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>264</v>
+      </c>
+      <c r="B80" t="s">
+        <v>260</v>
+      </c>
+      <c r="C80" t="s">
+        <v>261</v>
+      </c>
+      <c r="E80">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>264</v>
+      </c>
+      <c r="B81" t="s">
+        <v>259</v>
+      </c>
+      <c r="C81" t="s">
+        <v>261</v>
+      </c>
+      <c r="E81">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>264</v>
+      </c>
+      <c r="B82" t="s">
+        <v>259</v>
+      </c>
+      <c r="C82" t="s">
+        <v>261</v>
+      </c>
+      <c r="E82">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>265</v>
+      </c>
+      <c r="B83" t="s">
+        <v>262</v>
+      </c>
+      <c r="C83" t="s">
+        <v>261</v>
+      </c>
+      <c r="E83">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B84" t="s">
+        <v>263</v>
+      </c>
+      <c r="C84" t="s">
+        <v>261</v>
+      </c>
+      <c r="E84">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B85" t="s">
+        <v>266</v>
+      </c>
+      <c r="C85" t="s">
+        <v>267</v>
+      </c>
+      <c r="E85">
+        <v>973449.13247599336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>